<commit_message>
Update SAM ToDo and Beta feedback spreadsheets
</commit_message>
<xml_diff>
--- a/sam-2014-beta-feedback.xlsx
+++ b/sam-2014-beta-feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="180">
   <si>
     <t>Date</t>
   </si>
@@ -632,6 +632,12 @@
   </si>
   <si>
     <t>Replied with cc to Janine. Should be addressed by new Wind Farm layout option</t>
+  </si>
+  <si>
+    <t>Stephen.Frank@nrel.gov</t>
+  </si>
+  <si>
+    <t>Request to make it easier to transfer sam inputs to SDK -- enhancements to inputs browser</t>
   </si>
 </sst>
 </file>
@@ -1007,11 +1013,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E56" sqref="E56"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,6 +2194,23 @@
       </c>
       <c r="F55" s="1">
         <v>41929</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>41934</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>178</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F56" s="1">
+        <v>41934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update beta feedback spreadsheet oct 23
</commit_message>
<xml_diff>
--- a/sam-2014-beta-feedback.xlsx
+++ b/sam-2014-beta-feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="189">
   <si>
     <t>Date</t>
   </si>
@@ -638,6 +638,35 @@
   </si>
   <si>
     <t>Request to make it easier to transfer sam inputs to SDK -- enhancements to inputs browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here is the model I would like to simulate.  The model has 208 modules on the flat roof and  70 on the pitched roof.  I modeled this building looks like two but actually it is just one building; so, just one electricity meter.  At least two different string inverters are needed.
+I believe that, for this situation, multiple subsystem modeling feature is much useful.
+</t>
+  </si>
+  <si>
+    <t>.  I am attaching two screen shots; one is for SAM 2014.1.14  and another is for SAM 2014.9.30.  For PG&amp;E residential, usually it is monthly tier but on new SAM 2014.9.30, there is no monthly tiers.</t>
+  </si>
+  <si>
+    <t>Usability issue with URDB window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ‘register’ button didn’t look like a button. </t>
+  </si>
+  <si>
+    <t>Michael F. Troge &lt;mtroge@oneidanation.org&gt;</t>
+  </si>
+  <si>
+    <t>Followed up. Forwarded to team.</t>
+  </si>
+  <si>
+    <t>Followed up. On meeting agenda.</t>
+  </si>
+  <si>
+    <t>Will  the new version be able to load saved zsam files from the previous version, or TMY.tm2 weather files downloaded in the previous version?</t>
+  </si>
+  <si>
+    <t>Gomez, Tommaso &lt;tommaso.gomez@intel.com&gt;</t>
   </si>
 </sst>
 </file>
@@ -1013,11 +1042,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,7 +2079,7 @@
       </c>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>41926</v>
       </c>
@@ -2071,7 +2100,7 @@
       </c>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>41928</v>
       </c>
@@ -2092,7 +2121,7 @@
       </c>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>41928</v>
       </c>
@@ -2113,7 +2142,7 @@
       </c>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>41928</v>
       </c>
@@ -2134,7 +2163,7 @@
       </c>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>41928</v>
       </c>
@@ -2155,7 +2184,7 @@
       </c>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>41928</v>
       </c>
@@ -2176,7 +2205,7 @@
       </c>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>41929</v>
       </c>
@@ -2196,7 +2225,7 @@
         <v>41929</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>41934</v>
       </c>
@@ -2211,6 +2240,89 @@
       </c>
       <c r="F56" s="1">
         <v>41934</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>41935</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F57" s="1">
+        <v>41935</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>41933</v>
+      </c>
+      <c r="B58" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F58" s="1">
+        <v>41933</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>41933</v>
+      </c>
+      <c r="B59" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" t="s">
+        <v>184</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F59" s="1">
+        <v>41933</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>41933</v>
+      </c>
+      <c r="B60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F60" s="1">
+        <v>41933</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update beta feedback list #other #none
</commit_message>
<xml_diff>
--- a/sam-2014-beta-feedback.xlsx
+++ b/sam-2014-beta-feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="195">
   <si>
     <t>Date</t>
   </si>
@@ -667,6 +667,32 @@
   </si>
   <si>
     <t>Gomez, Tommaso &lt;tommaso.gomez@intel.com&gt;</t>
+  </si>
+  <si>
+    <t>Followed upPaul, we don't have the time to do scripting, what we are looking for is sample reports like what are available in PVSyst. I agree that it would be useful to provide the report editor available but you will get lots of request for assistance since scripting knowledge is required. 
+Also when under the 'Electric Load' tab you get the error below
+Could not evaluate callback function:visualize_load_data-&gt;on_change
+[2]: failed to evaluate function call argument 6 to 'dview()'
+Concerning the need for load;
+The part that doesn't make sense to me is how to set the parameters for large projects that we have no load, just generation. there is a rate plan we have input and the value of the power changes with the load size. so we have to create a load profile that is large enough to use the generation.
+Our buy rate is $0.00 because we are generation only. I have attached the project, If you look at Option A Fixed, that profile has the load set to 0. Please help</t>
+  </si>
+  <si>
+    <t>Emailed to Janine</t>
+  </si>
+  <si>
+    <t>the help data for 'performance model outputs' under "Results" does not work
+Also 'Time dependent Pricing Overview' also comes up with a "Page Not Found" error</t>
+  </si>
+  <si>
+    <t>1) In the parametric analysis, the results don't necessarily respond to changes in the main simulation.  In other words, let's say the parametric run tests the effect of different 5 different analysis periods.  I run the main simulation, then run the parametric simulation, no problem.  Now let's say I change the financing terms in the main simulation, and want to re-run the parametric test.  The only way to get it to run again is to change the value in each of the parametric input cells to something different, then change it back.  Alternatively, the number of cells can be decreased (wiping them out), and then increased back.  If I don't do that, re-running the parametric simulation will not produce results that reflect the change in financing that I had entered into the main simulation.
+2) The other more minor one that catches me is the inability to specify strings of uneven lengths, when using the advanced residential system design.  Using the "Number of strings in parallel" seems to require the strings to be of the same size.  The alternative using the PV Array Sizing Calculator Algorithm doesn't seem to work well at all, at least in the &lt; 10 kW residential systems I've attempted to model.  It might help if the size field accepted decimal point entry.</t>
+  </si>
+  <si>
+    <t>Forwarded to Aron and Steve to fix parametrics issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jason Sensibaugh' &lt;sensij@yahoo.com&gt; </t>
   </si>
 </sst>
 </file>
@@ -1042,11 +1068,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,9 +1081,10 @@
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" customWidth="1"/>
     <col min="4" max="4" width="71.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1740,7 +1767,7 @@
       </c>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>41912</v>
       </c>
@@ -1761,7 +1788,7 @@
       </c>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>41912</v>
       </c>
@@ -1785,7 +1812,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>41912</v>
       </c>
@@ -1799,14 +1826,20 @@
         <v>101</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>66</v>
+        <v>189</v>
       </c>
       <c r="F35" s="1">
         <v>41918</v>
       </c>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G35" s="7"/>
+      <c r="H35" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I35" s="1">
+        <v>41939</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>41912</v>
       </c>
@@ -1827,7 +1860,7 @@
       </c>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>41912</v>
       </c>
@@ -1848,7 +1881,7 @@
       </c>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>41907</v>
       </c>
@@ -1872,7 +1905,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>41896</v>
       </c>
@@ -1893,7 +1926,7 @@
       </c>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>41919</v>
       </c>
@@ -1914,7 +1947,7 @@
       </c>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41919</v>
       </c>
@@ -1935,7 +1968,7 @@
       </c>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41915</v>
       </c>
@@ -1956,7 +1989,7 @@
       </c>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41911</v>
       </c>
@@ -1980,7 +2013,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>41920</v>
       </c>
@@ -2001,7 +2034,7 @@
       </c>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41921</v>
       </c>
@@ -2022,7 +2055,7 @@
       </c>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>41922</v>
       </c>
@@ -2040,7 +2073,7 @@
       </c>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>41926</v>
       </c>
@@ -2061,7 +2094,7 @@
       </c>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>41926</v>
       </c>
@@ -2324,6 +2357,48 @@
       <c r="F60" s="1">
         <v>41933</v>
       </c>
+    </row>
+    <row r="61" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>41939</v>
+      </c>
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" t="s">
+        <v>102</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F61" s="1">
+        <v>41939</v>
+      </c>
+      <c r="G61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>41939</v>
+      </c>
+      <c r="B62" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F62" s="1">
+        <v>41939</v>
+      </c>
+      <c r="G62" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
update beta feedback spreadsheet #other
</commit_message>
<xml_diff>
--- a/sam-2014-beta-feedback.xlsx
+++ b/sam-2014-beta-feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="211">
   <si>
     <t>Date</t>
   </si>
@@ -693,6 +693,66 @@
   </si>
   <si>
     <t xml:space="preserve">Jason Sensibaugh' &lt;sensij@yahoo.com&gt; </t>
+  </si>
+  <si>
+    <t>Hi, this looks good, particularly improved shade modelling and sub-hourly PV simulations. However I haven’t been able to run a proper trial as I am stuck on the data input. I tried to use a TMY3 file that I created in SAM 2014.1.14 but in SAM beta it crashes. It has -99 values for some parameters (pressure, dewpoint) which may be the cause? I couldn’t find the TMY3 editor/creator functionality – is this not yet implemented in SAM beta?
+I also could not find any way to load a “USER” CEC module that I had created. Is this functionality not yet implemented in SAM beta?
+Some other comments: 
+·         Array setup, “Array” diagram would be useful
+·         Pre inverter derate “Nameplate” needs to allow negative loss for case of positive tolerance</t>
+  </si>
+  <si>
+    <t>Simon Faulkner &lt;Simon.Faulkner@aurecongroup.com&gt;</t>
+  </si>
+  <si>
+    <t>Forwarded request for negative derates to Janine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.       When I first launch SAM Beta it says it will expire in 29 days. If I enter the key I register will it still expire in 29days?
+2.       We deploy software out in our lab based on Symantec ghost imaging. I build one computer, install all the software and image it out. Will the key work still after I deploy out the software?
+3.       We run reduce user privilege in labs, all users have user level access with no administrative rights. We also use folder roaming/redirection to a network home drive (desktop, my docs, appdata, etc..). Will there be any issues?
+</t>
+  </si>
+  <si>
+    <t>Jason Chong &lt;jchong@engr.scu.edu&gt;</t>
+  </si>
+  <si>
+    <t>Forwarded to Aron and Steve. Potential issue with registration keys on ghost images because each copy has to be registererd</t>
+  </si>
+  <si>
+    <t>cash flow depreciation table pops out over cash flow.</t>
+  </si>
+  <si>
+    <t>Could not replicate. Forwarded to Steve and Aron. Asked for info about computer</t>
+  </si>
+  <si>
+    <t>Thanks for all the time you took to reply, I know your busy and taking the amount of time you did is greatly appreciated. We are using PVsyst for all our bankable projects but SAM is SO MUCH easier it would be nice to be able to use it for more applications. 
+Once the report editor is available I look forward to having the reporting edited and we will disperse the new reports to our dealer network. 
+Using the multipliers will make using SAM for generation projects a viable option at least initially.  Is there plans to use real rates and not multipliers?  The reason is our generation projects are huge and a small variation in rates causes the financials to be off a considerable percentage</t>
+  </si>
+  <si>
+    <t>Asked for clarification on energy market pricing request</t>
+  </si>
+  <si>
+    <t>I am currently using SAM to run multiple solar PV analyses at different locations.
+After about 12 locations (the maximum visible on the top SAM ribbon), additional cases can be created but they cannot later be accessed. i.e. 
+the only cases which can be accessed are those visible in the top ribbon.
+Good work on the upgrades.</t>
+  </si>
+  <si>
+    <t>Thomas Conroy &lt;tconroy@evolving-energy.com&gt;</t>
+  </si>
+  <si>
+    <t>Added explanation to Help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jason Sensibaugh &lt;sensij@yahoo.com&gt; </t>
+  </si>
+  <si>
+    <t>SAM does not account for debt liability after analysis period but allows debt period to be longer than analysis period.</t>
+  </si>
+  <si>
+    <t>Added warning message to UI</t>
   </si>
 </sst>
 </file>
@@ -1068,11 +1128,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1215,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>41899</v>
       </c>
@@ -2175,7 +2235,7 @@
       </c>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>41928</v>
       </c>
@@ -2399,6 +2459,128 @@
         <v>41939</v>
       </c>
       <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>41941</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F63" s="1">
+        <v>41941</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>41941</v>
+      </c>
+      <c r="B64" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" t="s">
+        <v>199</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F64" s="1">
+        <v>41941</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>41941</v>
+      </c>
+      <c r="B65" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" t="s">
+        <v>102</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F65" s="1">
+        <v>41941</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>41941</v>
+      </c>
+      <c r="B66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F66" s="1">
+        <v>41941</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>41941</v>
+      </c>
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" t="s">
+        <v>206</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F67" s="1">
+        <v>41941</v>
+      </c>
+      <c r="G67" s="5"/>
+    </row>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>41941</v>
+      </c>
+      <c r="B68" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" t="s">
+        <v>208</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F68" s="1">
+        <v>41941</v>
+      </c>
+      <c r="G68" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
update beta feedback workbook
</commit_message>
<xml_diff>
--- a/sam-2014-beta-feedback.xlsx
+++ b/sam-2014-beta-feedback.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="223">
   <si>
     <t>Date</t>
   </si>
@@ -483,9 +483,6 @@
     <t>Forwarded to Aron and Steve. Potential issue with registration keys on ghost images because each copy has to be registererd</t>
   </si>
   <si>
-    <t>cash flow depreciation table pops out over cash flow.</t>
-  </si>
-  <si>
     <t>Could not replicate. Forwarded to Steve and Aron. Asked for info about computer</t>
   </si>
   <si>
@@ -510,9 +507,6 @@
     <t>Hobbs, Will &lt;WHOBBS@southernco.com&gt;</t>
   </si>
   <si>
-    <t>Asked for copy of file</t>
-  </si>
-  <si>
     <t>Need to resolve before release</t>
   </si>
   <si>
@@ -523,9 +517,6 @@
   </si>
   <si>
     <t>Huisenga, Mike D. &lt;mike.huisenga@wspgroup.com&gt;</t>
-  </si>
-  <si>
-    <t>#1 may be a bug -- sent to Steve. #2 not really a problem -- need to document.</t>
   </si>
   <si>
     <t>Johannes Fehr &lt;johannes.fehr@ifeu.de&gt;</t>
@@ -754,6 +745,34 @@
   </si>
   <si>
     <t>Fixed.</t>
+  </si>
+  <si>
+    <t>One more issue, when I tried to add a newer module than is in your database I used the "CEC Performance Model with User ..." and when I tried to calculate and plot i get the error below., I also attached the screenshot showing the values we used. 
+Could not evaluate callback function:btnCalcIVCurve-&gt;on_change
+[7]: reference to unassigned variable: isc
+[7]: !error: access violation to non-numeric data</t>
+  </si>
+  <si>
+    <t>Fixed error in UI callback. (changed isc and voc variables to refer to input variable names)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cash flow depreciation table pops out over cash flow.
+Jut using a simple HP desktop standard, we ran into it on another desktop that is a DELL but she just restarted it and didnt see it again..  We never ran into it on any other computer running the current version. The table is just written on the screen, it is not selectable, and if I select any of the table it rewrites the screen to show just what should be there. but since I can not select the first column the screen is not usable, if I close and reopen it is fine. </t>
+  </si>
+  <si>
+    <t>One more change, can you sort the rate plans alphabetically?  Trying to find the right TOU for Southern California Edison. Trying to find TOU GS-3 Option R and it is difficult because the list is all jumbled. 
+Talking about opening "Search For Rates"
+Enter Southern California Edison
+look at the list, it is painful to find the correct one.</t>
+  </si>
+  <si>
+    <t>Forwarded to Steve.</t>
+  </si>
+  <si>
+    <t>#1 may be a bug -- sent to Steve. #2 not really a problem -- need to document. #2 fixed by steve.</t>
+  </si>
+  <si>
+    <t>Asked for copy of file. Have set of files for testing. They can use new SAM CSV format with their "macro"</t>
   </si>
 </sst>
 </file>
@@ -1142,11 +1161,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1248,7 @@
       </c>
       <c r="G3" s="3"/>
       <c r="I3" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1255,7 +1274,7 @@
       </c>
       <c r="G4" s="3"/>
       <c r="I4" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1281,7 +1300,7 @@
       </c>
       <c r="G5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1342,7 +1361,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>26</v>
@@ -1402,10 +1421,10 @@
         <v>35</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F11" s="7">
         <v>41915</v>
@@ -1423,7 +1442,7 @@
         <v>36</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>37</v>
@@ -1486,10 +1505,10 @@
         <v>44</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F15" s="7">
         <v>41915</v>
@@ -1528,7 +1547,7 @@
         <v>49</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>48</v>
@@ -1570,10 +1589,10 @@
         <v>53</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F19" s="7">
         <v>41919</v>
@@ -1629,7 +1648,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>104</v>
@@ -1669,7 +1688,7 @@
         <v>65</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>58</v>
@@ -1690,10 +1709,10 @@
         <v>39</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F25" s="7">
         <v>41918</v>
@@ -1711,7 +1730,7 @@
         <v>64</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>66</v>
@@ -1732,7 +1751,7 @@
         <v>57</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>69</v>
@@ -1753,10 +1772,10 @@
         <v>71</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F28" s="7">
         <v>41919</v>
@@ -1774,7 +1793,7 @@
         <v>72</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>73</v>
@@ -1903,13 +1922,13 @@
         <v>86</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G35" s="3"/>
       <c r="I35" s="1"/>
@@ -1946,10 +1965,10 @@
         <v>89</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F37" s="7">
         <v>41919</v>
@@ -1967,10 +1986,10 @@
         <v>90</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F38" s="7">
         <v>41919</v>
@@ -2030,7 +2049,7 @@
         <v>96</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>103</v>
@@ -2051,7 +2070,7 @@
         <v>97</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>99</v>
@@ -2072,10 +2091,10 @@
         <v>98</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F43" s="7">
         <v>41919</v>
@@ -2093,7 +2112,7 @@
         <v>100</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>107</v>
@@ -2114,7 +2133,7 @@
         <v>101</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>102</v>
@@ -2178,7 +2197,7 @@
         <v>118</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F48" s="7">
         <v>41926</v>
@@ -2217,7 +2236,7 @@
         <v>123</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>124</v>
@@ -2259,7 +2278,7 @@
         <v>128</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>129</v>
@@ -2301,7 +2320,7 @@
         <v>135</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>136</v>
@@ -2362,7 +2381,7 @@
         <v>25</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>145</v>
@@ -2386,7 +2405,7 @@
         <v>142</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F58" s="7">
         <v>41933</v>
@@ -2446,7 +2465,7 @@
         <v>86</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>58</v>
@@ -2467,7 +2486,7 @@
         <v>149</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>148</v>
@@ -2488,10 +2507,10 @@
         <v>150</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F63" s="7">
         <v>41941</v>
@@ -2509,7 +2528,7 @@
         <v>151</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>152</v>
@@ -2519,7 +2538,7 @@
       </c>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>41941</v>
       </c>
@@ -2530,13 +2549,13 @@
         <v>86</v>
       </c>
       <c r="D65" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E65" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="F65" s="7">
-        <v>41941</v>
+        <v>41949</v>
       </c>
       <c r="G65" s="3"/>
     </row>
@@ -2551,10 +2570,10 @@
         <v>86</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F66" s="7">
         <v>41941</v>
@@ -2569,13 +2588,13 @@
         <v>14</v>
       </c>
       <c r="C67" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E67" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="F67" s="7">
         <v>41941</v>
@@ -2590,13 +2609,13 @@
         <v>34</v>
       </c>
       <c r="C68" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="E68" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="F68" s="7">
         <v>41941</v>
@@ -2611,18 +2630,18 @@
         <v>34</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>162</v>
+        <v>222</v>
       </c>
       <c r="F69" s="7">
-        <v>41942</v>
-      </c>
-      <c r="G69" s="5"/>
+        <v>41948</v>
+      </c>
+      <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
@@ -2632,18 +2651,18 @@
         <v>14</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>167</v>
+        <v>221</v>
       </c>
       <c r="F70" s="7">
-        <v>41942</v>
-      </c>
-      <c r="G70" s="5"/>
+        <v>41948</v>
+      </c>
+      <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
@@ -2653,13 +2672,13 @@
         <v>20</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F71" s="7">
         <v>41942</v>
@@ -2674,18 +2693,60 @@
         <v>14</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F72" s="7">
         <v>41942</v>
       </c>
       <c r="G72" s="5"/>
+    </row>
+    <row r="73" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>41948</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F73" s="1">
+        <v>41948</v>
+      </c>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>41948</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F74" s="1">
+        <v>41948</v>
+      </c>
+      <c r="G74" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
update sam beta feedback spreadsheet
</commit_message>
<xml_diff>
--- a/sam-2014-beta-feedback.xlsx
+++ b/sam-2014-beta-feedback.xlsx
@@ -1165,7 +1165,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2704,7 +2704,7 @@
       <c r="F72" s="7">
         <v>41942</v>
       </c>
-      <c r="G72" s="5"/>
+      <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A73" s="1">

</xml_diff>

<commit_message>
update beta feedback list
</commit_message>
<xml_diff>
--- a/sam-2014-beta-feedback.xlsx
+++ b/sam-2014-beta-feedback.xlsx
@@ -766,13 +766,13 @@
 look at the list, it is painful to find the correct one.</t>
   </si>
   <si>
-    <t>Forwarded to Steve.</t>
-  </si>
-  <si>
     <t>#1 may be a bug -- sent to Steve. #2 not really a problem -- need to document. #2 fixed by steve.</t>
   </si>
   <si>
     <t>Asked for copy of file. Have set of files for testing. They can use new SAM CSV format with their "macro"</t>
+  </si>
+  <si>
+    <t>Forwarded to Steve. Aron implemented filters.</t>
   </si>
 </sst>
 </file>
@@ -1163,9 +1163,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D74" sqref="A74:XFD74"/>
+      <selection pane="bottomLeft" activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,7 +2636,7 @@
         <v>176</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F69" s="7">
         <v>41948</v>
@@ -2657,7 +2657,7 @@
         <v>177</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F70" s="7">
         <v>41948</v>
@@ -2741,12 +2741,12 @@
         <v>219</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F74" s="1">
-        <v>41948</v>
-      </c>
-      <c r="G74" s="4"/>
+        <v>41949</v>
+      </c>
+      <c r="G74" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>